<commit_message>
With results length baffle test
</commit_message>
<xml_diff>
--- a/Results_LengthBaffle.xlsx
+++ b/Results_LengthBaffle.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="LengthBaffle" sheetId="2" r:id="rId1"/>
+    <sheet name="oud" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>LengthBaffle</t>
   </si>
@@ -66,6 +67,51 @@
   </si>
   <si>
     <t>velocity (U_IN) 0.1</t>
+  </si>
+  <si>
+    <t>velocity (U_IN) 0.2</t>
+  </si>
+  <si>
+    <t>0.1 NPJ</t>
+  </si>
+  <si>
+    <t>0.15 NPJ</t>
+  </si>
+  <si>
+    <t>0.2 NPJ</t>
+  </si>
+  <si>
+    <t>0.25 NPJ</t>
+  </si>
+  <si>
+    <t>0.3 NPJ</t>
+  </si>
+  <si>
+    <t>0.35 NPJ</t>
+  </si>
+  <si>
+    <t>0.4 NPJ</t>
+  </si>
+  <si>
+    <t>0.45 NPJ</t>
+  </si>
+  <si>
+    <t>0.5 NPJ</t>
+  </si>
+  <si>
+    <t>0.55 NPJ</t>
+  </si>
+  <si>
+    <t>0.6 NPJ</t>
+  </si>
+  <si>
+    <t>0.65 NPJ</t>
+  </si>
+  <si>
+    <t>0.7 NPJ</t>
+  </si>
+  <si>
+    <t>Convergeerde niet, steeds 100 iteraties</t>
   </si>
 </sst>
 </file>
@@ -97,10 +143,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -109,9 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -392,18 +449,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="E2">
+        <v>-3.7400000000000003E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.501</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.375</v>
+      </c>
+      <c r="E3">
+        <v>-3.8800000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.502</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="E4">
+        <v>-4.07E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.503</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>0.313</v>
+      </c>
+      <c r="E5">
+        <v>-4.3299999999999998E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.503</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E6">
+        <v>-4.6600000000000003E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.503</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="E7">
+        <v>-5.1200000000000002E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.502</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="E8">
+        <v>-5.7299999999999997E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>0.17</v>
+      </c>
+      <c r="E9">
+        <v>-6.5600000000000006E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="E10">
+        <v>-7.7200000000000005E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>0.115</v>
+      </c>
+      <c r="E11">
+        <v>-9.35E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="E12">
+        <v>-0.11700000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -422,23 +786,30 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="2"/>
       <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="U1" t="s">
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,14 +828,21 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" t="s">
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="W2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,14 +861,21 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="R3">
+        <v>18</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,14 +894,21 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
         <v>8</v>
       </c>
-      <c r="U4" t="s">
+      <c r="R4">
+        <v>24</v>
+      </c>
+      <c r="W4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -535,14 +927,39 @@
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L5">
+        <v>-0.183</v>
+      </c>
+      <c r="M5">
+        <v>0.505</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="R5">
+        <v>30</v>
+      </c>
+      <c r="S5">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="T5">
+        <v>-0.191</v>
+      </c>
+      <c r="U5">
+        <v>0.505</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -558,8 +975,24 @@
       <c r="E6">
         <v>0.50700000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="I6" s="2"/>
+      <c r="J6">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="L6">
+        <v>-0.218</v>
+      </c>
+      <c r="M6">
+        <v>0.502</v>
+      </c>
+      <c r="R6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -575,8 +1008,24 @@
       <c r="E7">
         <v>0.50700000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="I7" s="2"/>
+      <c r="J7">
+        <v>28</v>
+      </c>
+      <c r="K7">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="L7">
+        <v>-0.248</v>
+      </c>
+      <c r="M7">
+        <v>0.501</v>
+      </c>
+      <c r="R7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -592,8 +1041,15 @@
       <c r="E8">
         <v>0.50600000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="I8" s="2"/>
+      <c r="J8">
+        <v>32</v>
+      </c>
+      <c r="R8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -609,8 +1065,15 @@
       <c r="E9">
         <v>0.504</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="I9" s="2"/>
+      <c r="J9">
+        <v>36</v>
+      </c>
+      <c r="R9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -626,26 +1089,15 @@
       <c r="E10">
         <v>0.503</v>
       </c>
+      <c r="I10" s="2"/>
       <c r="J10">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="K10">
-        <v>-0.19600000000000001</v>
-      </c>
-      <c r="L10">
-        <v>0.503</v>
-      </c>
-      <c r="Q10">
-        <v>0.436</v>
+        <v>40</v>
       </c>
       <c r="R10">
-        <v>-0.127</v>
-      </c>
-      <c r="S10">
-        <v>0.502</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -655,17 +1107,24 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
+      <c r="I11" s="2"/>
       <c r="J11">
+        <v>44</v>
+      </c>
+      <c r="K11">
         <v>0.30599999999999999</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>-0.20599999999999999</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.503</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -675,17 +1134,15 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
+      <c r="I12" s="2"/>
       <c r="J12">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="K12">
-        <v>-0.218</v>
-      </c>
-      <c r="L12">
-        <v>0.502</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="R12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -695,17 +1152,24 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
+      <c r="I13" s="2"/>
       <c r="J13">
+        <v>52</v>
+      </c>
+      <c r="K13">
         <v>0.25900000000000001</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>-0.23200000000000001</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.502</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -715,17 +1179,18 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
+      <c r="I14" s="2"/>
       <c r="J14">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="K14">
-        <v>-0.248</v>
-      </c>
-      <c r="L14">
-        <v>0.501</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="R14">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
@@ -738,44 +1203,45 @@
       <c r="G16" t="s">
         <v>4</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I16" s="2"/>
+      <c r="K16" t="s">
         <v>2</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>3</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>6</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>4</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>2</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>3</v>
       </c>
-      <c r="S16" t="s">
+      <c r="U16" t="s">
         <v>6</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
         <v>4</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>2</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AA16" t="s">
         <v>3</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AB16" t="s">
         <v>6</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>6.4399999999999999E-2</v>
       </c>
@@ -788,75 +1254,97 @@
       <c r="G17" t="s">
         <v>5</v>
       </c>
-      <c r="J17">
+      <c r="I17" s="2"/>
+      <c r="K17">
         <v>0.16500000000000001</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>-1.5599999999999999E-2</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>0.49399999999999999</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>5</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>0.183</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>-1.3299999999999999E-2</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>0.49299999999999999</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
         <v>5</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AD17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:30" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="I18" s="2"/>
+      <c r="O18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:30" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="N19" t="s">
+      <c r="I19" s="2"/>
+      <c r="O19" t="s">
         <v>8</v>
       </c>
-      <c r="U19" t="s">
+      <c r="W19" t="s">
         <v>8</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:30" x14ac:dyDescent="0.3">
       <c r="G20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="I20" s="2"/>
+      <c r="O20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="W20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="21" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="I26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>